<commit_message>
update r code for processing incoming data
</commit_message>
<xml_diff>
--- a/dokumentation/project_layout/fr_en_text_ids.xlsx
+++ b/dokumentation/project_layout/fr_en_text_ids.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherchandler/repo/Python/computerlinguistik/de_np_kongru/dokumentation/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherchandler/repo/Python/computerlinguistik/de_np_kongru/dokumentation/project_layout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A1CF59-F387-C044-95E3-2616CCB0290F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289FF2C8-6E08-5240-8391-5C66024D5FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2B5DE780-DB4A-8948-9369-D4AE7FDCE00B}"/>
+    <workbookView xWindow="38340" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2B5DE780-DB4A-8948-9369-D4AE7FDCE00B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -341,18 +341,12 @@
       <name val=".AppleSystemUIFont"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -376,8 +370,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,52 +689,53 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="J2" sqref="J2:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="30.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18" style="2" customWidth="1"/>
+    <col min="10" max="10" width="30.1640625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -751,10 +746,10 @@
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -783,10 +778,10 @@
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -803,13 +798,13 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -826,13 +821,13 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -849,19 +844,19 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>58</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -872,168 +867,168 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="17" spans="8:8">
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="8:8">
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="8:8">
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="8:8">
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="3" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update documentation.docx Run test texts
</commit_message>
<xml_diff>
--- a/dokumentation/project_layout/fr_en_text_ids.xlsx
+++ b/dokumentation/project_layout/fr_en_text_ids.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherchandler/repo/Python/computerlinguistik/de_np_kongru/dokumentation/project_layout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289FF2C8-6E08-5240-8391-5C66024D5FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC134D4-E55C-9848-B599-59FE6C89FDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38340" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2B5DE780-DB4A-8948-9369-D4AE7FDCE00B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2B5DE780-DB4A-8948-9369-D4AE7FDCE00B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -327,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -340,8 +340,20 @@
       <color rgb="FF000000"/>
       <name val=".AppleSystemUIFont"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val=".AppleSystemUIFont"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,6 +363,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,11 +385,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,53 +710,52 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J6"/>
+      <selection activeCell="B5" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18" style="2" customWidth="1"/>
-    <col min="10" max="10" width="30.1640625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -746,10 +766,10 @@
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -778,10 +798,10 @@
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="6" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -804,7 +824,7 @@
       <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -827,7 +847,7 @@
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -844,19 +864,19 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="6" t="s">
         <v>58</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -867,168 +887,169 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="B10" s="4"/>
+      <c r="E10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="6" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="17" spans="8:8">
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="8:8">
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="8:8">
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="8:8">
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>